<commit_message>
dev IHM - tests calibration
</commit_message>
<xml_diff>
--- a/01_doc/Fichier csv test résultats - boîte à moustaches.xlsx
+++ b/01_doc/Fichier csv test résultats - boîte à moustaches.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Julien\Stage_1DOF_DroneBench\01_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D2075A-0E31-424F-BC8A-FB5B054A2B36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94713311-9319-4D43-B6D1-D5C21A4B36EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4568A270-C64E-45CB-9E9D-852ADEFA779F}"/>
   </bookViews>
@@ -21,10 +21,6 @@
     <definedName name="_xlchart.v1.1" hidden="1">GFG!$B$3:$B$272</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">GFG!$A$3:$A$272</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">GFG!$B$3:$B$272</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">GFG!$B$3:$B$272</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">GFG!$C$3:$C$272</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">GFG!$A$3:$A$272</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">GFG!$B$3:$B$272</definedName>
     <definedName name="DonnéesExternes_1" localSheetId="0" hidden="1">GFG!$A$1:$A$272</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -160,9 +156,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -190,10 +185,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.7</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -231,8 +226,8 @@
         <cx:series layoutId="boxWhisker" uniqueId="{C8E48E8E-DFB9-4498-BEE7-B8DE6C79F571}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="0" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
+            <cx:visibility meanLine="1" meanMarker="0" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="inclusive"/>
           </cx:layoutPr>
         </cx:series>
       </cx:plotAreaRegion>
@@ -854,7 +849,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="3688080" y="426720"/>
+              <a:off x="2895600" y="426720"/>
               <a:ext cx="6774180" cy="4225290"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1211,7 +1206,7 @@
   <dimension ref="A1:B272"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1228,2170 +1223,2170 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>27.141131000000001</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>17.860555000000002</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>9.9037550000000003</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>4.3271540000000002</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>1.0513300000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>-0.76866500000000004</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>-1.6184559999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>-1.7326269999999999</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>-1.5859780000000001</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>-1.2177020000000001</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>-0.89754199999999995</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>-0.51911300000000005</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>-0.16484599999999999</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>0.271698</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0.57604599999999995</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>3.4957769999999999</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>3.042529</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>4.866428</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>3.7072690000000001</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>3.3015379999999999</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>4.8941920000000003</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>5.9753420000000004</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>6.3376239999999999</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>7.2807310000000003</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>8.2359109999999998</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>8.2005459999999992</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>6.9126329999999996</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>5.3949959999999999</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>4.5989190000000004</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>5.1293949999999997</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B33" s="2">
+      <c r="B33" s="1">
         <v>4.3588279999999999</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="1">
         <v>8.4551639999999999</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B35" s="2">
+      <c r="B35" s="1">
         <v>6.1192789999999997</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="1">
         <v>8.8833459999999995</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B37" s="2">
+      <c r="B37" s="1">
         <v>8.8960869999999996</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2">
+      <c r="B38" s="1">
         <v>9.5106439999999992</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B39" s="1">
         <v>12.974797000000001</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="1">
         <v>14.369854</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B41" s="2">
+      <c r="B41" s="1">
         <v>15.655056</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B42" s="2">
+      <c r="B42" s="1">
         <v>12.135903000000001</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B43" s="2">
+      <c r="B43" s="1">
         <v>9.3242779999999996</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="2">
+      <c r="B44" s="1">
         <v>9.2607879999999998</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="1">
         <v>9.0747250000000008</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B46" s="2">
+      <c r="B46" s="1">
         <v>7.7217359999999999</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="1">
         <v>7.6070960000000003</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="1">
         <v>6.2213529999999997</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>5.3549519999999999</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="1">
         <v>6.718146</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="2">
+      <c r="B51" s="1">
         <v>6.2713929999999998</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="1">
         <v>7.4321489999999999</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="1">
         <v>10.626132</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="2" t="s">
+      <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="2">
+      <c r="B54" s="1">
         <v>13.299305</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B55" s="2">
+      <c r="B55" s="1">
         <v>15.245075999999999</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B56" s="2">
+      <c r="B56" s="1">
         <v>14.641919</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="1">
         <v>12.466825999999999</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="1">
         <v>15.462987999999999</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="1">
         <v>12.995112000000001</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
+      <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B60" s="2">
+      <c r="B60" s="1">
         <v>13.140324</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="1">
         <v>11.477899000000001</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>10.625935</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="1">
         <v>10.452230999999999</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>8.8597739999999998</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="2" t="s">
+      <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B65" s="2">
+      <c r="B65" s="1">
         <v>9.6751760000000004</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
+      <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="1">
         <v>7.7143750000000004</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
+      <c r="A67" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="1">
         <v>17.721662999999999</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
+      <c r="A68" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B68" s="2">
+      <c r="B68" s="1">
         <v>24.791620999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
+      <c r="A69" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B69" s="1">
         <v>34.058996</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A70" s="2" t="s">
+      <c r="A70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B70" s="2">
+      <c r="B70" s="1">
         <v>31.652567000000001</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B71" s="1">
         <v>39.763486999999998</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="1">
         <v>45.029411000000003</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B73" s="1">
         <v>40.873711999999998</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B74" s="2">
+      <c r="B74" s="1">
         <v>34.801056000000003</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B75" s="2">
+      <c r="B75" s="1">
         <v>32.497169</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="1">
         <v>26.809916999999999</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="s">
+      <c r="A77" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B77" s="2">
+      <c r="B77" s="1">
         <v>28.453735999999999</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B78" s="2">
+      <c r="B78" s="1">
         <v>29.289269000000001</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A79" s="2" t="s">
+      <c r="A79" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B79" s="2">
+      <c r="B79" s="1">
         <v>31.141736000000002</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="1">
         <v>26.324641</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="1">
         <v>32.500303000000002</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B82" s="2">
+      <c r="B82" s="1">
         <v>36.166611000000003</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+      <c r="A83" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B83" s="2">
+      <c r="B83" s="1">
         <v>32.580022999999997</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A84" s="2" t="s">
+      <c r="A84" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B84" s="2">
+      <c r="B84" s="1">
         <v>28.082605000000001</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A85" s="2" t="s">
+      <c r="A85" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B85" s="2">
+      <c r="B85" s="1">
         <v>25.258389999999999</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A86" s="2" t="s">
+      <c r="A86" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B86" s="2">
+      <c r="B86" s="1">
         <v>24.773793000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A87" s="2" t="s">
+      <c r="A87" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B87" s="2">
+      <c r="B87" s="1">
         <v>25.398503000000002</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
+      <c r="A88" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B88" s="2">
+      <c r="B88" s="1">
         <v>21.776641000000001</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A89" s="2" t="s">
+      <c r="A89" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B89" s="2">
+      <c r="B89" s="1">
         <v>21.110496000000001</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A90" s="2" t="s">
+      <c r="A90" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B90" s="2">
+      <c r="B90" s="1">
         <v>20.044170000000001</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A91" s="2" t="s">
+      <c r="A91" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B91" s="2">
+      <c r="B91" s="1">
         <v>16.133506000000001</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A92" s="2" t="s">
+      <c r="A92" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B92" s="2">
+      <c r="B92" s="1">
         <v>17.226721999999999</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
+      <c r="A93" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B93" s="2">
+      <c r="B93" s="1">
         <v>18.675826000000001</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A94" s="2" t="s">
+      <c r="A94" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B94" s="2">
+      <c r="B94" s="1">
         <v>18.780106</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A95" s="2" t="s">
+      <c r="A95" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B95" s="2">
+      <c r="B95" s="1">
         <v>21.237252999999999</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A96" s="2" t="s">
+      <c r="A96" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B96" s="2">
+      <c r="B96" s="1">
         <v>18.212038</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="2" t="s">
+      <c r="A97" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B97" s="2">
+      <c r="B97" s="1">
         <v>19.126550999999999</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A98" s="2" t="s">
+      <c r="A98" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B98" s="2">
+      <c r="B98" s="1">
         <v>19.931460000000001</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A99" s="2" t="s">
+      <c r="A99" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B99" s="2">
+      <c r="B99" s="1">
         <v>17.843340000000001</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B100" s="2">
+      <c r="B100" s="1">
         <v>17.787506</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A101" s="2" t="s">
+      <c r="A101" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B101" s="2">
+      <c r="B101" s="1">
         <v>21.890452</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+      <c r="A102" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B102" s="2">
+      <c r="B102" s="1">
         <v>20.011809</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A103" s="2" t="s">
+      <c r="A103" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B103" s="2">
+      <c r="B103" s="1">
         <v>19.108754000000001</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A104" s="2" t="s">
+      <c r="A104" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B104" s="2">
+      <c r="B104" s="1">
         <v>19.822282000000001</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A105" s="2" t="s">
+      <c r="A105" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B105" s="2">
+      <c r="B105" s="1">
         <v>17.682748</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A106" s="2" t="s">
+      <c r="A106" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B106" s="2">
+      <c r="B106" s="1">
         <v>19.844401999999999</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A107" s="2" t="s">
+      <c r="A107" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B107" s="2">
+      <c r="B107" s="1">
         <v>18.583022</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A108" s="2" t="s">
+      <c r="A108" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B108" s="2">
+      <c r="B108" s="1">
         <v>18.186263</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A109" s="2" t="s">
+      <c r="A109" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B109" s="2">
+      <c r="B109" s="1">
         <v>21.104879</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A110" s="2" t="s">
+      <c r="A110" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B110" s="2">
+      <c r="B110" s="1">
         <v>19.578527999999999</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A111" s="2" t="s">
+      <c r="A111" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B111" s="2">
+      <c r="B111" s="1">
         <v>19.479716</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A112" s="2" t="s">
+      <c r="A112" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B112" s="2">
+      <c r="B112" s="1">
         <v>18.244176</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A113" s="2" t="s">
+      <c r="A113" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B113" s="2">
+      <c r="B113" s="1">
         <v>18.833531000000001</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A114" s="2" t="s">
+      <c r="A114" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B114" s="2">
+      <c r="B114" s="1">
         <v>17.877600999999999</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A115" s="2" t="s">
+      <c r="A115" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B115" s="2">
+      <c r="B115" s="1">
         <v>19.715845000000002</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A116" s="2" t="s">
+      <c r="A116" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B116" s="2">
+      <c r="B116" s="1">
         <v>22.440681999999999</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A117" s="2" t="s">
+      <c r="A117" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B117" s="2">
+      <c r="B117" s="1">
         <v>21.871721999999998</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A118" s="2" t="s">
+      <c r="A118" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B118" s="2">
+      <c r="B118" s="1">
         <v>20.376871000000001</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A119" s="2" t="s">
+      <c r="A119" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B119" s="2">
+      <c r="B119" s="1">
         <v>20.686648000000002</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A120" s="2" t="s">
+      <c r="A120" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B120" s="2">
+      <c r="B120" s="1">
         <v>20.044751999999999</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A121" s="2" t="s">
+      <c r="A121" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B121" s="2">
+      <c r="B121" s="1">
         <v>18.588632</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A122" s="2" t="s">
+      <c r="A122" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B122" s="2">
+      <c r="B122" s="1">
         <v>19.226744</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A123" s="2" t="s">
+      <c r="A123" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B123" s="2">
+      <c r="B123" s="1">
         <v>19.249282999999998</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A124" s="2" t="s">
+      <c r="A124" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B124" s="2">
+      <c r="B124" s="1">
         <v>18.181688000000001</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A125" s="2" t="s">
+      <c r="A125" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B125" s="2">
+      <c r="B125" s="1">
         <v>18.351158000000002</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A126" s="2" t="s">
+      <c r="A126" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B126" s="2">
+      <c r="B126" s="1">
         <v>18.110835999999999</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A127" s="2" t="s">
+      <c r="A127" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B127" s="2">
+      <c r="B127" s="1">
         <v>19.280892999999999</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A128" s="2" t="s">
+      <c r="A128" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B128" s="2">
+      <c r="B128" s="1">
         <v>18.860316000000001</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A129" s="2" t="s">
+      <c r="A129" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B129" s="2">
+      <c r="B129" s="1">
         <v>20.063884999999999</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A130" s="2" t="s">
+      <c r="A130" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B130" s="2">
+      <c r="B130" s="1">
         <v>25.503181000000001</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A131" s="2" t="s">
+      <c r="A131" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B131" s="2">
+      <c r="B131" s="1">
         <v>25.490928</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A132" s="2" t="s">
+      <c r="A132" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B132" s="2">
+      <c r="B132" s="1">
         <v>23.283308000000002</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A133" s="2" t="s">
+      <c r="A133" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B133" s="2">
+      <c r="B133" s="1">
         <v>22.447073</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A134" s="2" t="s">
+      <c r="A134" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B134" s="2">
+      <c r="B134" s="1">
         <v>24.775535999999999</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A135" s="2" t="s">
+      <c r="A135" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B135" s="2">
+      <c r="B135" s="1">
         <v>24.448149000000001</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A136" s="2" t="s">
+      <c r="A136" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B136" s="2">
+      <c r="B136" s="1">
         <v>23.969145000000001</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A137" s="2" t="s">
+      <c r="A137" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B137" s="2">
+      <c r="B137" s="1">
         <v>25.236592000000002</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A138" s="2" t="s">
+      <c r="A138" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B138" s="2">
+      <c r="B138" s="1">
         <v>24.333307999999999</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A139" s="2" t="s">
+      <c r="A139" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B139" s="2">
+      <c r="B139" s="1">
         <v>25.023751000000001</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A140" s="2" t="s">
+      <c r="A140" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B140" s="2">
+      <c r="B140" s="1">
         <v>25.668044999999999</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A141" s="2" t="s">
+      <c r="A141" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B141" s="2">
+      <c r="B141" s="1">
         <v>27.235612</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A142" s="2" t="s">
+      <c r="A142" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B142" s="2">
+      <c r="B142" s="1">
         <v>25.806467999999999</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A143" s="2" t="s">
+      <c r="A143" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B143" s="2">
+      <c r="B143" s="1">
         <v>24.214393000000001</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A144" s="2" t="s">
+      <c r="A144" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B144" s="2">
+      <c r="B144" s="1">
         <v>23.829142000000001</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="2" t="s">
+      <c r="A145" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B145" s="2">
+      <c r="B145" s="1">
         <v>24.409022</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="2" t="s">
+      <c r="A146" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B146" s="2">
+      <c r="B146" s="1">
         <v>29.643146999999999</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="2" t="s">
+      <c r="A147" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B147" s="2">
+      <c r="B147" s="1">
         <v>31.377175999999999</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="2" t="s">
+      <c r="A148" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B148" s="2">
+      <c r="B148" s="1">
         <v>29.169195999999999</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="2" t="s">
+      <c r="A149" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B149" s="2">
+      <c r="B149" s="1">
         <v>28.392790999999999</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="2" t="s">
+      <c r="A150" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B150" s="2">
+      <c r="B150" s="1">
         <v>26.082939</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="2" t="s">
+      <c r="A151" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B151" s="2">
+      <c r="B151" s="1">
         <v>26.748239000000002</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="2" t="s">
+      <c r="A152" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B152" s="2">
+      <c r="B152" s="1">
         <v>26.150247</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="2" t="s">
+      <c r="A153" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B153" s="2">
+      <c r="B153" s="1">
         <v>27.521239999999999</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="2" t="s">
+      <c r="A154" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B154" s="2">
+      <c r="B154" s="1">
         <v>27.974656</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="2" t="s">
+      <c r="A155" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B155" s="2">
+      <c r="B155" s="1">
         <v>27.795100000000001</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="2" t="s">
+      <c r="A156" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B156" s="2">
+      <c r="B156" s="1">
         <v>28.178101999999999</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="2" t="s">
+      <c r="A157" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B157" s="2">
+      <c r="B157" s="1">
         <v>29.501134</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="2" t="s">
+      <c r="A158" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B158" s="2">
+      <c r="B158" s="1">
         <v>30.517748000000001</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="2" t="s">
+      <c r="A159" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B159" s="2">
+      <c r="B159" s="1">
         <v>30.216366000000001</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="2" t="s">
+      <c r="A160" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B160" s="2">
+      <c r="B160" s="1">
         <v>29.591263000000001</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="2" t="s">
+      <c r="A161" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B161" s="2">
+      <c r="B161" s="1">
         <v>31.414391999999999</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="2" t="s">
+      <c r="A162" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B162" s="2">
+      <c r="B162" s="1">
         <v>35.585054</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="2" t="s">
+      <c r="A163" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B163" s="2">
+      <c r="B163" s="1">
         <v>40.528055999999999</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="2" t="s">
+      <c r="A164" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B164" s="2">
+      <c r="B164" s="1">
         <v>39.356904999999998</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="2" t="s">
+      <c r="A165" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B165" s="2">
+      <c r="B165" s="1">
         <v>39.935589999999998</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="2" t="s">
+      <c r="A166" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B166" s="2">
+      <c r="B166" s="1">
         <v>41.475752</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="2" t="s">
+      <c r="A167" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B167" s="2">
+      <c r="B167" s="1">
         <v>40.210830000000001</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="2" t="s">
+      <c r="A168" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B168" s="2">
+      <c r="B168" s="1">
         <v>41.853515999999999</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="2" t="s">
+      <c r="A169" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B169" s="2">
+      <c r="B169" s="1">
         <v>42.226139000000003</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="2" t="s">
+      <c r="A170" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B170" s="2">
+      <c r="B170" s="1">
         <v>43.182980000000001</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="2" t="s">
+      <c r="A171" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B171" s="2">
+      <c r="B171" s="1">
         <v>40.068612000000002</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="2" t="s">
+      <c r="A172" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B172" s="2">
+      <c r="B172" s="1">
         <v>42.567393000000003</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="2" t="s">
+      <c r="A173" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B173" s="2">
+      <c r="B173" s="1">
         <v>40.641461</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="2" t="s">
+      <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B174" s="2">
+      <c r="B174" s="1">
         <v>38.602989999999998</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="2" t="s">
+      <c r="A175" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B175" s="2">
+      <c r="B175" s="1">
         <v>38.502746999999999</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="2" t="s">
+      <c r="A176" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B176" s="2">
+      <c r="B176" s="1">
         <v>42.082042999999999</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="2" t="s">
+      <c r="A177" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B177" s="2">
+      <c r="B177" s="1">
         <v>40.889806</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="2" t="s">
+      <c r="A178" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B178" s="2">
+      <c r="B178" s="1">
         <v>40.650815999999999</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="2" t="s">
+      <c r="A179" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B179" s="2">
+      <c r="B179" s="1">
         <v>37.269508000000002</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="2" t="s">
+      <c r="A180" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B180" s="2">
+      <c r="B180" s="1">
         <v>38.433067999999999</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="2" t="s">
+      <c r="A181" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B181" s="2">
+      <c r="B181" s="1">
         <v>37.159919000000002</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="2" t="s">
+      <c r="A182" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B182" s="2">
+      <c r="B182" s="1">
         <v>37.873657999999999</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="2" t="s">
+      <c r="A183" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B183" s="2">
+      <c r="B183" s="1">
         <v>38.033574000000002</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="2" t="s">
+      <c r="A184" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B184" s="2">
+      <c r="B184" s="1">
         <v>39.800111999999999</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="2" t="s">
+      <c r="A185" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B185" s="2">
+      <c r="B185" s="1">
         <v>37.259686000000002</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="2" t="s">
+      <c r="A186" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B186" s="2">
+      <c r="B186" s="1">
         <v>37.297148999999997</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="2" t="s">
+      <c r="A187" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B187" s="2">
+      <c r="B187" s="1">
         <v>36.037582999999998</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="2" t="s">
+      <c r="A188" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B188" s="2">
+      <c r="B188" s="1">
         <v>37.143892000000001</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="2" t="s">
+      <c r="A189" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B189" s="2">
+      <c r="B189" s="1">
         <v>35.785611000000003</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="2" t="s">
+      <c r="A190" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B190" s="2">
+      <c r="B190" s="1">
         <v>36.098866000000001</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="2" t="s">
+      <c r="A191" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B191" s="2">
+      <c r="B191" s="1">
         <v>37.468018999999998</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="2" t="s">
+      <c r="A192" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B192" s="2">
+      <c r="B192" s="1">
         <v>37.196184000000002</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="2" t="s">
+      <c r="A193" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B193" s="2">
+      <c r="B193" s="1">
         <v>47.113793000000001</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="2" t="s">
+      <c r="A194" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B194" s="2">
+      <c r="B194" s="1">
         <v>50.114218000000001</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="2" t="s">
+      <c r="A195" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B195" s="2">
+      <c r="B195" s="1">
         <v>48.428289999999997</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="2" t="s">
+      <c r="A196" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B196" s="2">
+      <c r="B196" s="1">
         <v>44.110551000000001</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="2" t="s">
+      <c r="A197" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B197" s="2">
+      <c r="B197" s="1">
         <v>41.417726000000002</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="2" t="s">
+      <c r="A198" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B198" s="2">
+      <c r="B198" s="1">
         <v>40.080362999999998</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="2" t="s">
+      <c r="A199" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B199" s="2">
+      <c r="B199" s="1">
         <v>39.586568999999997</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="2" t="s">
+      <c r="A200" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B200" s="2">
+      <c r="B200" s="1">
         <v>39.190522000000001</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="2" t="s">
+      <c r="A201" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B201" s="2">
+      <c r="B201" s="1">
         <v>41.450211000000003</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="2" t="s">
+      <c r="A202" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B202" s="2">
+      <c r="B202" s="1">
         <v>40.139220999999999</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="2" t="s">
+      <c r="A203" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B203" s="2">
+      <c r="B203" s="1">
         <v>40.428477000000001</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="2" t="s">
+      <c r="A204" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B204" s="2">
+      <c r="B204" s="1">
         <v>40.057586000000001</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="2" t="s">
+      <c r="A205" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B205" s="2">
+      <c r="B205" s="1">
         <v>42.160777000000003</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="2" t="s">
+      <c r="A206" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B206" s="2">
+      <c r="B206" s="1">
         <v>44.412708000000002</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="2" t="s">
+      <c r="A207" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B207" s="2">
+      <c r="B207" s="1">
         <v>44.375793000000002</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="2" t="s">
+      <c r="A208" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B208" s="2">
+      <c r="B208" s="1">
         <v>44.765811999999997</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="2" t="s">
+      <c r="A209" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B209" s="2">
+      <c r="B209" s="1">
         <v>45.106212999999997</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="2" t="s">
+      <c r="A210" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B210" s="2">
+      <c r="B210" s="1">
         <v>49.253812000000003</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="2" t="s">
+      <c r="A211" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B211" s="2">
+      <c r="B211" s="1">
         <v>52.041808000000003</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="2" t="s">
+      <c r="A212" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B212" s="2">
+      <c r="B212" s="1">
         <v>49.350771999999999</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="2" t="s">
+      <c r="A213" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B213" s="2">
+      <c r="B213" s="1">
         <v>50.022460000000002</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="2" t="s">
+      <c r="A214" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B214" s="2">
+      <c r="B214" s="1">
         <v>49.657083999999998</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="2" t="s">
+      <c r="A215" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B215" s="2">
+      <c r="B215" s="1">
         <v>50.977629</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="2" t="s">
+      <c r="A216" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B216" s="2">
+      <c r="B216" s="1">
         <v>51.346587</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="2" t="s">
+      <c r="A217" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B217" s="2">
+      <c r="B217" s="1">
         <v>50.542228999999999</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="2" t="s">
+      <c r="A218" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B218" s="2">
+      <c r="B218" s="1">
         <v>52.316338000000002</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="2" t="s">
+      <c r="A219" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B219" s="2">
+      <c r="B219" s="1">
         <v>51.805280000000003</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="2" t="s">
+      <c r="A220" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B220" s="2">
+      <c r="B220" s="1">
         <v>51.403930000000003</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="2" t="s">
+      <c r="A221" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B221" s="2">
+      <c r="B221" s="1">
         <v>52.127851</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="2" t="s">
+      <c r="A222" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B222" s="2">
+      <c r="B222" s="1">
         <v>52.155805000000001</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="2" t="s">
+      <c r="A223" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B223" s="2">
+      <c r="B223" s="1">
         <v>50.860306999999999</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="2" t="s">
+      <c r="A224" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B224" s="2">
+      <c r="B224" s="1">
         <v>50.468597000000003</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="2" t="s">
+      <c r="A225" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B225" s="2">
+      <c r="B225" s="1">
         <v>50.428767999999998</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="2" t="s">
+      <c r="A226" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B226" s="2">
+      <c r="B226" s="1">
         <v>56.305295999999998</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="2" t="s">
+      <c r="A227" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B227" s="2">
+      <c r="B227" s="1">
         <v>60.085369</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="2" t="s">
+      <c r="A228" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B228" s="2">
+      <c r="B228" s="1">
         <v>57.799788999999997</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="2" t="s">
+      <c r="A229" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B229" s="2">
+      <c r="B229" s="1">
         <v>55.960639</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="2" t="s">
+      <c r="A230" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B230" s="2">
+      <c r="B230" s="1">
         <v>56.839830999999997</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="2" t="s">
+      <c r="A231" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B231" s="2">
+      <c r="B231" s="1">
         <v>58.716206999999997</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="2" t="s">
+      <c r="A232" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B232" s="2">
+      <c r="B232" s="1">
         <v>58.295994999999998</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="2" t="s">
+      <c r="A233" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B233" s="2">
+      <c r="B233" s="1">
         <v>58.660777000000003</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="2" t="s">
+      <c r="A234" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B234" s="2">
+      <c r="B234" s="1">
         <v>59.100712000000001</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="2" t="s">
+      <c r="A235" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B235" s="2">
+      <c r="B235" s="1">
         <v>59.725417999999998</v>
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="2" t="s">
+      <c r="A236" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B236" s="2">
+      <c r="B236" s="1">
         <v>59.395949000000002</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="2" t="s">
+      <c r="A237" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B237" s="2">
+      <c r="B237" s="1">
         <v>59.432355000000001</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="2" t="s">
+      <c r="A238" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B238" s="2">
+      <c r="B238" s="1">
         <v>59.574134999999998</v>
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="2" t="s">
+      <c r="A239" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B239" s="2">
+      <c r="B239" s="1">
         <v>59.163946000000003</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="2" t="s">
+      <c r="A240" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B240" s="2">
+      <c r="B240" s="1">
         <v>61.117398000000001</v>
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="2" t="s">
+      <c r="A241" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B241" s="2">
+      <c r="B241" s="1">
         <v>65.041916999999998</v>
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="2" t="s">
+      <c r="A242" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B242" s="2">
+      <c r="B242" s="1">
         <v>66.801981999999995</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="2" t="s">
+      <c r="A243" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B243" s="2">
+      <c r="B243" s="1">
         <v>70.194153</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="2" t="s">
+      <c r="A244" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B244" s="2">
+      <c r="B244" s="1">
         <v>69.437735000000004</v>
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="2" t="s">
+      <c r="A245" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B245" s="2">
+      <c r="B245" s="1">
         <v>69.657463000000007</v>
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="2" t="s">
+      <c r="A246" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B246" s="2">
+      <c r="B246" s="1">
         <v>70.923339999999996</v>
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="2" t="s">
+      <c r="A247" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B247" s="2">
+      <c r="B247" s="1">
         <v>72.249167</v>
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="2" t="s">
+      <c r="A248" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B248" s="2">
+      <c r="B248" s="1">
         <v>75.183497000000003</v>
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="2" t="s">
+      <c r="A249" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B249" s="2">
+      <c r="B249" s="1">
         <v>75.507686000000007</v>
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="2" t="s">
+      <c r="A250" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B250" s="2">
+      <c r="B250" s="1">
         <v>69.703228999999993</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="2" t="s">
+      <c r="A251" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B251" s="2">
+      <c r="B251" s="1">
         <v>69.955706000000006</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="2" t="s">
+      <c r="A252" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B252" s="2">
+      <c r="B252" s="1">
         <v>70.588149000000001</v>
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="2" t="s">
+      <c r="A253" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B253" s="2">
+      <c r="B253" s="1">
         <v>70.409380999999996</v>
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="2" t="s">
+      <c r="A254" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B254" s="2">
+      <c r="B254" s="1">
         <v>68.317335</v>
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="2" t="s">
+      <c r="A255" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B255" s="2">
+      <c r="B255" s="1">
         <v>68.841700000000003</v>
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="2" t="s">
+      <c r="A256" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B256" s="2">
+      <c r="B256" s="1">
         <v>67.370159999999998</v>
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="2" t="s">
+      <c r="A257" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B257" s="2">
+      <c r="B257" s="1">
         <v>67.410321999999994</v>
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="2" t="s">
+      <c r="A258" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B258" s="2">
+      <c r="B258" s="1">
         <v>73.464770999999999</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="2" t="s">
+      <c r="A259" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B259" s="2">
+      <c r="B259" s="1">
         <v>64.929276999999999</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="2" t="s">
+      <c r="A260" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B260" s="2">
+      <c r="B260" s="1">
         <v>67.303675999999996</v>
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="2" t="s">
+      <c r="A261" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B261" s="2">
+      <c r="B261" s="1">
         <v>67.835094999999995</v>
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="2" t="s">
+      <c r="A262" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B262" s="2">
+      <c r="B262" s="1">
         <v>69.585006000000007</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="2" t="s">
+      <c r="A263" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B263" s="2">
+      <c r="B263" s="1">
         <v>71.980710000000002</v>
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="2" t="s">
+      <c r="A264" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B264" s="2">
+      <c r="B264" s="1">
         <v>70.843830999999994</v>
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="2" t="s">
+      <c r="A265" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B265" s="2">
+      <c r="B265" s="1">
         <v>72.845371</v>
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="2" t="s">
+      <c r="A266" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B266" s="2">
+      <c r="B266" s="1">
         <v>74.005336</v>
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="2" t="s">
+      <c r="A267" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B267" s="2">
+      <c r="B267" s="1">
         <v>74.268045000000001</v>
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="2" t="s">
+      <c r="A268" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B268" s="2">
+      <c r="B268" s="1">
         <v>73.156712999999996</v>
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="2" t="s">
+      <c r="A269" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B269" s="2">
+      <c r="B269" s="1">
         <v>75.008267000000004</v>
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="2" t="s">
+      <c r="A270" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B270" s="2">
+      <c r="B270" s="1">
         <v>76.260377000000005</v>
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="2" t="s">
+      <c r="A271" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B271" s="2">
+      <c r="B271" s="1">
         <v>76.477807999999996</v>
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="2" t="s">
+      <c r="A272" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B272" s="2">
+      <c r="B272" s="1">
         <v>77.320525000000004</v>
       </c>
     </row>

</xml_diff>